<commit_message>
Updated csv to support local species and location
</commit_message>
<xml_diff>
--- a/resources/IBP_Filled_In_Template.xlsx
+++ b/resources/IBP_Filled_In_Template.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\OneDrive\Documents\udemy\C#Learning\SnatchIt\Core\SnatchItCore\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A854C26E-45D6-4216-BD10-2FB682F8587F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7345A0-FCB9-4FCE-9FFF-014989A16ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="gsyKKuzBo0q13ZS+VgXqMrUoPpBOit2TyxAryVmYAgfXWL7g6YZklgfo6dgSZ0Iw/zf1XClxdVLTN4DRI6y4rA==" workbookSaltValue="S39lodf8WzQuRmjNJN1JpA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2655" yWindow="2640" windowWidth="25830" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Banding Data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="140">
   <si>
     <t>LOC</t>
   </si>
@@ -249,9 +249,6 @@
     <t>JC</t>
   </si>
   <si>
-    <t>DUFL</t>
-  </si>
-  <si>
     <t>PS</t>
   </si>
   <si>
@@ -306,27 +303,15 @@
     <t>C</t>
   </si>
   <si>
-    <t>LAZB</t>
-  </si>
-  <si>
     <t>DEFG</t>
   </si>
   <si>
     <t>ABCD</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>NM</t>
-  </si>
-  <si>
     <t>0A</t>
   </si>
   <si>
-    <t>NAWA</t>
-  </si>
-  <si>
     <t>JS</t>
   </si>
   <si>
@@ -441,9 +426,6 @@
     <t>820</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>8</t>
   </si>
   <si>
@@ -463,6 +445,9 @@
   </si>
   <si>
     <t>times, nets, and notes with a leading zero.</t>
+  </si>
+  <si>
+    <t>MORS</t>
   </si>
 </sst>
 </file>
@@ -854,9 +839,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AH26" sqref="AH26:AH30"/>
+      <selection pane="bottomLeft" activeCell="AM5" sqref="AM5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,7 +992,7 @@
     </row>
     <row r="2" spans="1:39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>71</v>
@@ -1016,7 +1001,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>71</v>
@@ -1025,22 +1010,22 @@
         <v>287081451</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H2" s="12">
         <v>5</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="K2" s="12" t="s">
         <v>13</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M2" s="12">
         <v>6</v>
@@ -1058,29 +1043,29 @@
         <v>0</v>
       </c>
       <c r="R2" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S2" s="12">
         <v>3</v>
       </c>
       <c r="T2" s="12"/>
       <c r="U2" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="V2" s="12" t="s">
         <v>13</v>
       </c>
       <c r="W2" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="X2" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Y2" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z2" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA2" s="12"/>
       <c r="AB2" s="12"/>
@@ -1097,10 +1082,10 @@
         <v>44350</v>
       </c>
       <c r="AG2" s="12" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="AH2" s="12" t="s">
-        <v>93</v>
+        <v>139</v>
       </c>
       <c r="AI2" s="12">
         <v>10</v>
@@ -1112,7 +1097,7 @@
     </row>
     <row r="3" spans="1:39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>71</v>
@@ -1121,7 +1106,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>71</v>
@@ -1130,22 +1115,22 @@
         <v>272127720</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="H3" s="12">
         <v>6</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K3" s="12" t="s">
         <v>13</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M3" s="12">
         <v>6</v>
@@ -1163,29 +1148,29 @@
         <v>0</v>
       </c>
       <c r="R3" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S3" s="12">
         <v>3</v>
       </c>
       <c r="T3" s="12"/>
       <c r="U3" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V3" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="W3" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="X3" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Y3" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Z3" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AA3" s="12"/>
       <c r="AB3" s="12"/>
@@ -1202,13 +1187,13 @@
         <v>44350</v>
       </c>
       <c r="AG3" s="12" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="AH3" s="12" t="s">
-        <v>93</v>
+        <v>139</v>
       </c>
       <c r="AI3" s="12" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="AJ3" s="12"/>
       <c r="AK3" s="12"/>
@@ -1217,7 +1202,7 @@
     </row>
     <row r="4" spans="1:39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>71</v>
@@ -1226,7 +1211,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>71</v>
@@ -1235,16 +1220,16 @@
         <v>281149622</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="H4" s="12">
         <v>6</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K4" s="12" t="s">
         <v>13</v>
@@ -1268,29 +1253,29 @@
         <v>0</v>
       </c>
       <c r="R4" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S4" s="12">
         <v>3</v>
       </c>
       <c r="T4" s="12"/>
       <c r="U4" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V4" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="W4" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="X4" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Y4" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Z4" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AA4" s="12"/>
       <c r="AB4" s="12"/>
@@ -1307,13 +1292,13 @@
         <v>44354</v>
       </c>
       <c r="AG4" s="12" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="AH4" s="12" t="s">
-        <v>93</v>
+        <v>139</v>
       </c>
       <c r="AI4" s="12" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="AJ4" s="12"/>
       <c r="AK4" s="12">
@@ -1321,45 +1306,43 @@
       </c>
       <c r="AL4" s="12"/>
       <c r="AM4" s="12" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C5" s="12">
         <v>1</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="F5" s="12">
-        <v>287081580</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="F5" s="12"/>
       <c r="G5" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H5" s="12">
         <v>6</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K5" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="L5" s="12" t="s">
         <v>88</v>
-      </c>
-      <c r="L5" s="12" t="s">
-        <v>89</v>
       </c>
       <c r="M5" s="12">
         <v>6</v>
@@ -1377,29 +1360,29 @@
         <v>0</v>
       </c>
       <c r="R5" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S5" s="12">
         <v>3</v>
       </c>
       <c r="T5" s="12"/>
       <c r="U5" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V5" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="W5" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="X5" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Y5" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Z5" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AA5" s="12"/>
       <c r="AB5" s="12"/>
@@ -1410,64 +1393,62 @@
         <v>9.6</v>
       </c>
       <c r="AE5" s="12" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="AF5" s="11">
         <v>44362</v>
       </c>
       <c r="AG5" s="12" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="AH5" s="12" t="s">
-        <v>93</v>
+        <v>139</v>
       </c>
       <c r="AI5" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="AJ5" s="12" t="s">
-        <v>95</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="AJ5" s="12"/>
       <c r="AK5" s="12">
         <v>3</v>
       </c>
       <c r="AL5" s="12"/>
       <c r="AM5" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
       <c r="B6" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="12">
+        <v>1</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="12">
-        <v>1</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>102</v>
-      </c>
       <c r="E6" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F6" s="12">
         <v>291037530</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="H6" s="12">
         <v>5</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L6" s="12"/>
       <c r="M6" s="12">
@@ -1486,29 +1467,29 @@
         <v>0</v>
       </c>
       <c r="R6" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S6" s="12">
         <v>3</v>
       </c>
       <c r="T6" s="12"/>
       <c r="U6" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="V6" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="V6" s="12" t="s">
-        <v>83</v>
-      </c>
       <c r="W6" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="X6" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Y6" s="12" t="s">
         <v>13</v>
       </c>
       <c r="Z6" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA6" s="12"/>
       <c r="AB6" s="12"/>
@@ -1525,10 +1506,10 @@
         <v>44350</v>
       </c>
       <c r="AG6" s="12" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="AH6" s="12" t="s">
-        <v>93</v>
+        <v>139</v>
       </c>
       <c r="AI6" s="12">
         <v>10</v>
@@ -1540,37 +1521,37 @@
     </row>
     <row r="7" spans="1:39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
       <c r="B7" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="12">
+        <v>1</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C7" s="12">
-        <v>1</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>102</v>
-      </c>
       <c r="E7" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F7" s="12">
         <v>291037531</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="H7" s="12">
         <v>1</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L7" s="12"/>
       <c r="M7" s="12">
@@ -1599,13 +1580,13 @@
         <v>44372</v>
       </c>
       <c r="AG7" s="12" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="AH7" s="12" t="s">
-        <v>93</v>
+        <v>139</v>
       </c>
       <c r="AI7" s="12" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="AJ7" s="12"/>
       <c r="AK7" s="12">
@@ -1613,45 +1594,45 @@
       </c>
       <c r="AL7" s="12"/>
       <c r="AM7" s="12" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
       <c r="B8" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="12">
+        <v>1</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C8" s="12">
-        <v>1</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>102</v>
-      </c>
       <c r="E8" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F8" s="12">
         <v>291037532</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="H8" s="12">
         <v>6</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K8" s="12" t="s">
         <v>13</v>
       </c>
       <c r="L8" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M8" s="12">
         <v>6</v>
@@ -1669,29 +1650,29 @@
         <v>0</v>
       </c>
       <c r="R8" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S8" s="12">
         <v>5</v>
       </c>
       <c r="T8" s="12"/>
       <c r="U8" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V8" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="W8" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="X8" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Y8" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Z8" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AA8" s="12"/>
       <c r="AB8" s="12"/>
@@ -1708,13 +1689,13 @@
         <v>44372</v>
       </c>
       <c r="AG8" s="12" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="AH8" s="12" t="s">
-        <v>93</v>
+        <v>139</v>
       </c>
       <c r="AI8" s="12" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="AJ8" s="12"/>
       <c r="AK8" s="12"/>
@@ -1723,40 +1704,40 @@
     </row>
     <row r="9" spans="1:39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C9" s="12">
         <v>1</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F9" s="12">
         <v>291037533</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="H9" s="12">
         <v>2</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K9" s="12" t="s">
         <v>13</v>
       </c>
       <c r="L9" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M9" s="12">
         <v>2</v>
@@ -1774,7 +1755,7 @@
         <v>4</v>
       </c>
       <c r="R9" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S9" s="12">
         <v>1</v>
@@ -1783,28 +1764,28 @@
         <v>1</v>
       </c>
       <c r="U9" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="V9" s="12" t="s">
         <v>13</v>
       </c>
       <c r="W9" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="X9" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Y9" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z9" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA9" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AB9" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AC9" s="12">
         <v>56</v>
@@ -1819,10 +1800,10 @@
         <v>44393</v>
       </c>
       <c r="AG9" s="12" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="AH9" s="12" t="s">
-        <v>93</v>
+        <v>139</v>
       </c>
       <c r="AI9" s="12">
         <v>10</v>
@@ -1834,43 +1815,43 @@
     </row>
     <row r="10" spans="1:39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C10" s="12">
         <v>1</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F10" s="12">
         <v>291037534</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="H10" s="12">
         <v>2</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L10" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="N10" s="12">
         <v>0</v>
@@ -1882,34 +1863,34 @@
         <v>1</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="R10" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S10" s="12" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="T10" s="12">
         <v>1</v>
       </c>
       <c r="U10" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="V10" s="12" t="s">
         <v>13</v>
       </c>
       <c r="W10" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="X10" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Y10" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z10" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AA10" s="12"/>
       <c r="AB10" s="12"/>
@@ -1926,13 +1907,13 @@
         <v>44393</v>
       </c>
       <c r="AG10" s="12" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AH10" s="12" t="s">
-        <v>93</v>
+        <v>139</v>
       </c>
       <c r="AI10" s="12" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="AJ10" s="12"/>
       <c r="AK10" s="12"/>
@@ -1941,7 +1922,7 @@
     </row>
     <row r="11" spans="1:39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
       <c r="B11" s="12">
         <v>0</v>
@@ -1953,28 +1934,28 @@
         <v>72</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F11" s="12">
         <v>288070406</v>
       </c>
       <c r="G11" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="H11" s="12">
+        <v>1</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="L11" s="12" t="s">
         <v>90</v>
-      </c>
-      <c r="H11" s="12">
-        <v>1</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="K11" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="L11" s="12" t="s">
-        <v>91</v>
       </c>
       <c r="M11" s="12">
         <v>6</v>
@@ -1992,32 +1973,32 @@
         <v>0</v>
       </c>
       <c r="R11" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S11" s="12">
         <v>5</v>
       </c>
       <c r="T11" s="12"/>
       <c r="U11" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="V11" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="W11" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="X11" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y11" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z11" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA11" s="12" t="s">
         <v>75</v>
-      </c>
-      <c r="V11" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="W11" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="X11" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="Y11" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z11" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA11" s="12" t="s">
-        <v>76</v>
       </c>
       <c r="AB11" s="12"/>
       <c r="AC11" s="12">
@@ -2033,13 +2014,13 @@
         <v>44364</v>
       </c>
       <c r="AG11" s="12" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="AH11" s="12" t="s">
-        <v>93</v>
+        <v>139</v>
       </c>
       <c r="AI11" s="12" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="AJ11" s="12"/>
       <c r="AK11" s="12">
@@ -2047,12 +2028,12 @@
       </c>
       <c r="AL11" s="12"/>
       <c r="AM11" s="12" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
       <c r="B12" s="12">
         <v>0</v>
@@ -2061,31 +2042,31 @@
         <v>2</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F12" s="12">
         <v>288070409</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H12" s="12">
         <v>6</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K12" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="L12" s="12" t="s">
         <v>88</v>
-      </c>
-      <c r="L12" s="12" t="s">
-        <v>89</v>
       </c>
       <c r="M12" s="12">
         <v>6</v>
@@ -2103,29 +2084,29 @@
         <v>0</v>
       </c>
       <c r="R12" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S12" s="12">
         <v>3</v>
       </c>
       <c r="T12" s="12"/>
       <c r="U12" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V12" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="W12" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="X12" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Y12" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Z12" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AA12" s="12"/>
       <c r="AB12" s="12"/>
@@ -2139,44 +2120,44 @@
         <v>44383</v>
       </c>
       <c r="AG12" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="AH12" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="AI12" s="12" t="s">
         <v>134</v>
-      </c>
-      <c r="AH12" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="AI12" s="12" t="s">
-        <v>140</v>
       </c>
       <c r="AJ12" s="12"/>
       <c r="AK12" s="12"/>
       <c r="AL12" s="12"/>
       <c r="AM12" s="12" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="M15" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="M16" s="2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M17" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M18" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2238,10 +2219,10 @@
     </row>
     <row r="2" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C2" s="11">
         <v>44352</v>
@@ -2250,10 +2231,10 @@
         <v>4</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G2" s="12">
         <v>1</v>
@@ -2267,10 +2248,10 @@
     </row>
     <row r="3" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C3" s="11">
         <v>44352</v>
@@ -2279,7 +2260,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F3" s="12">
         <v>2</v>
@@ -2296,10 +2277,10 @@
     </row>
     <row r="4" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C4" s="11">
         <v>44352</v>
@@ -2308,7 +2289,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F4" s="12">
         <v>3</v>
@@ -2325,10 +2306,10 @@
     </row>
     <row r="5" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C5" s="11">
         <v>44352</v>
@@ -2337,7 +2318,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F5" s="12">
         <v>4</v>
@@ -2354,10 +2335,10 @@
     </row>
     <row r="6" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C6" s="11">
         <v>44352</v>
@@ -2366,7 +2347,7 @@
         <v>4</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F6" s="12">
         <v>5</v>
@@ -2383,10 +2364,10 @@
     </row>
     <row r="7" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C7" s="11">
         <v>44352</v>
@@ -2395,7 +2376,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F7" s="12">
         <v>6</v>
@@ -2412,10 +2393,10 @@
     </row>
     <row r="8" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C8" s="11">
         <v>44352</v>
@@ -2424,7 +2405,7 @@
         <v>4</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F8" s="12">
         <v>7</v>
@@ -2441,10 +2422,10 @@
     </row>
     <row r="9" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C9" s="11">
         <v>44352</v>
@@ -2453,7 +2434,7 @@
         <v>4</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F9" s="12">
         <v>8</v>
@@ -2470,10 +2451,10 @@
     </row>
     <row r="10" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C10" s="11">
         <v>44352</v>
@@ -2482,7 +2463,7 @@
         <v>4</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F10" s="12">
         <v>9</v>
@@ -2499,10 +2480,10 @@
     </row>
     <row r="11" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C11" s="11">
         <v>44352</v>
@@ -2511,7 +2492,7 @@
         <v>4</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F11" s="12">
         <v>10</v>
@@ -2528,10 +2509,10 @@
     </row>
     <row r="12" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C12" s="11">
         <v>44353</v>
@@ -2540,10 +2521,10 @@
         <v>4</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G12" s="12">
         <v>1</v>
@@ -2557,10 +2538,10 @@
     </row>
     <row r="13" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C13" s="11">
         <v>44353</v>
@@ -2569,7 +2550,7 @@
         <v>4</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F13" s="12">
         <v>2</v>
@@ -2586,10 +2567,10 @@
     </row>
     <row r="14" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C14" s="11">
         <v>44353</v>
@@ -2598,7 +2579,7 @@
         <v>4</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F14" s="12">
         <v>3</v>
@@ -2615,10 +2596,10 @@
     </row>
     <row r="15" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C15" s="11">
         <v>44353</v>
@@ -2627,7 +2608,7 @@
         <v>4</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F15" s="12">
         <v>4</v>
@@ -2644,10 +2625,10 @@
     </row>
     <row r="16" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C16" s="11">
         <v>44353</v>
@@ -2656,7 +2637,7 @@
         <v>4</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F16" s="12">
         <v>5</v>
@@ -2673,10 +2654,10 @@
     </row>
     <row r="17" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C17" s="11">
         <v>44353</v>
@@ -2685,7 +2666,7 @@
         <v>4</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F17" s="12">
         <v>6</v>
@@ -2702,10 +2683,10 @@
     </row>
     <row r="18" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C18" s="11">
         <v>44353</v>
@@ -2714,7 +2695,7 @@
         <v>4</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F18" s="12">
         <v>7</v>
@@ -2731,10 +2712,10 @@
     </row>
     <row r="19" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C19" s="11">
         <v>44353</v>
@@ -2743,7 +2724,7 @@
         <v>4</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F19" s="12">
         <v>8</v>
@@ -2760,10 +2741,10 @@
     </row>
     <row r="20" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C20" s="11">
         <v>44353</v>
@@ -2772,7 +2753,7 @@
         <v>4</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F20" s="12">
         <v>9</v>
@@ -2789,10 +2770,10 @@
     </row>
     <row r="21" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C21" s="11">
         <v>44353</v>
@@ -2801,7 +2782,7 @@
         <v>4</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F21" s="12">
         <v>10</v>
@@ -2818,10 +2799,10 @@
     </row>
     <row r="22" spans="1:9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C22" s="11">
         <v>44362</v>
@@ -2830,7 +2811,7 @@
         <v>5</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F22" s="12">
         <v>1</v>
@@ -2847,10 +2828,10 @@
     </row>
     <row r="23" spans="1:9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C23" s="11">
         <v>44362</v>
@@ -2859,7 +2840,7 @@
         <v>5</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F23" s="12">
         <v>2</v>
@@ -2876,10 +2857,10 @@
     </row>
     <row r="24" spans="1:9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C24" s="11">
         <v>44362</v>
@@ -2888,7 +2869,7 @@
         <v>5</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F24" s="12">
         <v>3</v>
@@ -2905,10 +2886,10 @@
     </row>
     <row r="25" spans="1:9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C25" s="11">
         <v>44362</v>
@@ -2917,7 +2898,7 @@
         <v>5</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F25" s="12">
         <v>4</v>
@@ -2934,10 +2915,10 @@
     </row>
     <row r="26" spans="1:9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C26" s="11">
         <v>44362</v>
@@ -2946,7 +2927,7 @@
         <v>5</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F26" s="12">
         <v>5</v>
@@ -2963,10 +2944,10 @@
     </row>
     <row r="27" spans="1:9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C27" s="11">
         <v>44362</v>
@@ -2975,7 +2956,7 @@
         <v>5</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F27" s="12">
         <v>6</v>
@@ -2992,10 +2973,10 @@
     </row>
     <row r="28" spans="1:9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C28" s="11">
         <v>44362</v>
@@ -3004,7 +2985,7 @@
         <v>5</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F28" s="12">
         <v>10</v>
@@ -3021,10 +3002,10 @@
     </row>
     <row r="29" spans="1:9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C29" s="11">
         <v>44366</v>
@@ -3033,7 +3014,7 @@
         <v>5</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F29" s="12">
         <v>1</v>
@@ -3050,10 +3031,10 @@
     </row>
     <row r="30" spans="1:9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C30" s="11">
         <v>44366</v>
@@ -3062,7 +3043,7 @@
         <v>5</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F30" s="12">
         <v>2</v>
@@ -3079,10 +3060,10 @@
     </row>
     <row r="31" spans="1:9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C31" s="11">
         <v>44366</v>
@@ -3091,7 +3072,7 @@
         <v>5</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F31" s="12">
         <v>3</v>
@@ -3108,10 +3089,10 @@
     </row>
     <row r="32" spans="1:9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C32" s="11">
         <v>44366</v>
@@ -3120,7 +3101,7 @@
         <v>5</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F32" s="12">
         <v>4</v>
@@ -3137,10 +3118,10 @@
     </row>
     <row r="33" spans="1:9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C33" s="11">
         <v>44366</v>
@@ -3149,7 +3130,7 @@
         <v>5</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F33" s="12">
         <v>5</v>
@@ -3166,10 +3147,10 @@
     </row>
     <row r="34" spans="1:9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C34" s="11">
         <v>44366</v>
@@ -3178,7 +3159,7 @@
         <v>5</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F34" s="12">
         <v>6</v>
@@ -3195,10 +3176,10 @@
     </row>
     <row r="35" spans="1:9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C35" s="11">
         <v>44366</v>
@@ -3207,7 +3188,7 @@
         <v>5</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F35" s="12">
         <v>10</v>
@@ -3224,10 +3205,10 @@
     </row>
     <row r="36" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C36" s="11">
         <v>44372</v>
@@ -3236,7 +3217,7 @@
         <v>6</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F36" s="12">
         <v>1</v>
@@ -3253,10 +3234,10 @@
     </row>
     <row r="37" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C37" s="11">
         <v>44372</v>
@@ -3265,7 +3246,7 @@
         <v>6</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F37" s="12">
         <v>2</v>
@@ -3282,10 +3263,10 @@
     </row>
     <row r="38" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C38" s="11">
         <v>44372</v>
@@ -3294,7 +3275,7 @@
         <v>6</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F38" s="12">
         <v>3</v>
@@ -3311,10 +3292,10 @@
     </row>
     <row r="39" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C39" s="11">
         <v>44372</v>
@@ -3323,7 +3304,7 @@
         <v>6</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F39" s="12">
         <v>4</v>
@@ -3340,10 +3321,10 @@
     </row>
     <row r="40" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C40" s="11">
         <v>44372</v>
@@ -3352,7 +3333,7 @@
         <v>6</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F40" s="12">
         <v>5</v>
@@ -3369,10 +3350,10 @@
     </row>
     <row r="41" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C41" s="11">
         <v>44372</v>
@@ -3381,7 +3362,7 @@
         <v>6</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F41" s="12">
         <v>6</v>
@@ -3398,10 +3379,10 @@
     </row>
     <row r="42" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C42" s="11">
         <v>44372</v>
@@ -3410,7 +3391,7 @@
         <v>6</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F42" s="12">
         <v>7</v>
@@ -3427,10 +3408,10 @@
     </row>
     <row r="43" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C43" s="11">
         <v>44372</v>
@@ -3439,7 +3420,7 @@
         <v>6</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F43" s="12">
         <v>8</v>
@@ -3456,10 +3437,10 @@
     </row>
     <row r="44" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C44" s="11">
         <v>44372</v>
@@ -3468,7 +3449,7 @@
         <v>6</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F44" s="12">
         <v>9</v>
@@ -3485,10 +3466,10 @@
     </row>
     <row r="45" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C45" s="11">
         <v>44372</v>
@@ -3497,7 +3478,7 @@
         <v>6</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F45" s="12">
         <v>10</v>
@@ -3514,10 +3495,10 @@
     </row>
     <row r="46" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C46" s="11">
         <v>44383</v>
@@ -3526,7 +3507,7 @@
         <v>7</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F46" s="12">
         <v>1</v>
@@ -3543,10 +3524,10 @@
     </row>
     <row r="47" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C47" s="11">
         <v>44383</v>
@@ -3555,7 +3536,7 @@
         <v>7</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F47" s="12">
         <v>2</v>
@@ -3572,10 +3553,10 @@
     </row>
     <row r="48" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C48" s="11">
         <v>44383</v>
@@ -3584,7 +3565,7 @@
         <v>7</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F48" s="12">
         <v>3</v>
@@ -3601,10 +3582,10 @@
     </row>
     <row r="49" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C49" s="11">
         <v>44383</v>
@@ -3613,7 +3594,7 @@
         <v>7</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F49" s="12">
         <v>4</v>
@@ -3630,10 +3611,10 @@
     </row>
     <row r="50" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C50" s="11">
         <v>44383</v>
@@ -3642,7 +3623,7 @@
         <v>7</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F50" s="12">
         <v>5</v>
@@ -3659,10 +3640,10 @@
     </row>
     <row r="51" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C51" s="11">
         <v>44383</v>
@@ -3671,7 +3652,7 @@
         <v>7</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F51" s="12">
         <v>6</v>
@@ -3688,10 +3669,10 @@
     </row>
     <row r="52" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C52" s="11">
         <v>44383</v>
@@ -3700,7 +3681,7 @@
         <v>7</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F52" s="12">
         <v>7</v>
@@ -3717,10 +3698,10 @@
     </row>
     <row r="53" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C53" s="11">
         <v>44383</v>
@@ -3729,7 +3710,7 @@
         <v>7</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F53" s="12">
         <v>8</v>
@@ -3746,10 +3727,10 @@
     </row>
     <row r="54" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C54" s="11">
         <v>44383</v>
@@ -3758,7 +3739,7 @@
         <v>7</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F54" s="12">
         <v>9</v>
@@ -3775,10 +3756,10 @@
     </row>
     <row r="55" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C55" s="11">
         <v>44383</v>
@@ -3787,7 +3768,7 @@
         <v>7</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F55" s="12">
         <v>10</v>
@@ -3804,10 +3785,10 @@
     </row>
     <row r="56" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C56" s="11">
         <v>44393</v>
@@ -3816,7 +3797,7 @@
         <v>8</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F56" s="12">
         <v>1</v>
@@ -3833,10 +3814,10 @@
     </row>
     <row r="57" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C57" s="11">
         <v>44393</v>
@@ -3845,7 +3826,7 @@
         <v>8</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F57" s="12">
         <v>2</v>
@@ -3862,10 +3843,10 @@
     </row>
     <row r="58" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C58" s="11">
         <v>44393</v>
@@ -3874,7 +3855,7 @@
         <v>8</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F58" s="12">
         <v>3</v>
@@ -3891,10 +3872,10 @@
     </row>
     <row r="59" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C59" s="11">
         <v>44393</v>
@@ -3903,7 +3884,7 @@
         <v>8</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F59" s="12">
         <v>4</v>
@@ -3920,10 +3901,10 @@
     </row>
     <row r="60" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C60" s="11">
         <v>44393</v>
@@ -3932,7 +3913,7 @@
         <v>8</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F60" s="12">
         <v>5</v>
@@ -3949,10 +3930,10 @@
     </row>
     <row r="61" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C61" s="11">
         <v>44393</v>
@@ -3961,7 +3942,7 @@
         <v>8</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F61" s="12">
         <v>6</v>
@@ -3978,10 +3959,10 @@
     </row>
     <row r="62" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C62" s="11">
         <v>44393</v>
@@ -3990,7 +3971,7 @@
         <v>8</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F62" s="12">
         <v>7</v>
@@ -4007,10 +3988,10 @@
     </row>
     <row r="63" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C63" s="11">
         <v>44393</v>
@@ -4019,7 +4000,7 @@
         <v>8</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F63" s="12">
         <v>8</v>
@@ -4036,10 +4017,10 @@
     </row>
     <row r="64" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C64" s="11">
         <v>44393</v>
@@ -4048,7 +4029,7 @@
         <v>8</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F64" s="12">
         <v>9</v>
@@ -4065,10 +4046,10 @@
     </row>
     <row r="65" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C65" s="11">
         <v>44393</v>
@@ -4077,7 +4058,7 @@
         <v>8</v>
       </c>
       <c r="E65" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F65" s="12">
         <v>10</v>
@@ -4094,10 +4075,10 @@
     </row>
     <row r="66" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C66" s="11">
         <v>44401</v>
@@ -4106,7 +4087,7 @@
         <v>9</v>
       </c>
       <c r="E66" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F66" s="12">
         <v>1</v>
@@ -4123,10 +4104,10 @@
     </row>
     <row r="67" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C67" s="11">
         <v>44401</v>
@@ -4135,7 +4116,7 @@
         <v>9</v>
       </c>
       <c r="E67" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F67" s="12">
         <v>2</v>
@@ -4152,10 +4133,10 @@
     </row>
     <row r="68" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C68" s="11">
         <v>44401</v>
@@ -4164,7 +4145,7 @@
         <v>9</v>
       </c>
       <c r="E68" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F68" s="12">
         <v>3</v>
@@ -4181,10 +4162,10 @@
     </row>
     <row r="69" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C69" s="11">
         <v>44401</v>
@@ -4193,7 +4174,7 @@
         <v>9</v>
       </c>
       <c r="E69" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F69" s="12">
         <v>4</v>
@@ -4210,10 +4191,10 @@
     </row>
     <row r="70" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C70" s="11">
         <v>44401</v>
@@ -4222,7 +4203,7 @@
         <v>9</v>
       </c>
       <c r="E70" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F70" s="12">
         <v>5</v>
@@ -4239,10 +4220,10 @@
     </row>
     <row r="71" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C71" s="11">
         <v>44401</v>
@@ -4251,7 +4232,7 @@
         <v>9</v>
       </c>
       <c r="E71" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F71" s="12">
         <v>6</v>
@@ -4268,10 +4249,10 @@
     </row>
     <row r="72" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C72" s="11">
         <v>44401</v>
@@ -4280,7 +4261,7 @@
         <v>9</v>
       </c>
       <c r="E72" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F72" s="12">
         <v>7</v>
@@ -4297,10 +4278,10 @@
     </row>
     <row r="73" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B73" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C73" s="11">
         <v>44401</v>
@@ -4309,7 +4290,7 @@
         <v>9</v>
       </c>
       <c r="E73" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F73" s="12">
         <v>8</v>
@@ -4326,10 +4307,10 @@
     </row>
     <row r="74" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C74" s="11">
         <v>44401</v>
@@ -4338,7 +4319,7 @@
         <v>9</v>
       </c>
       <c r="E74" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F74" s="12">
         <v>9</v>
@@ -4355,10 +4336,10 @@
     </row>
     <row r="75" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B75" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C75" s="11">
         <v>44401</v>
@@ -4367,7 +4348,7 @@
         <v>9</v>
       </c>
       <c r="E75" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F75" s="12">
         <v>10</v>
@@ -4384,10 +4365,10 @@
     </row>
     <row r="76" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C76" s="11">
         <v>44411</v>
@@ -4396,7 +4377,7 @@
         <v>10</v>
       </c>
       <c r="E76" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F76" s="12">
         <v>1</v>
@@ -4413,10 +4394,10 @@
     </row>
     <row r="77" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C77" s="11">
         <v>44411</v>
@@ -4425,7 +4406,7 @@
         <v>10</v>
       </c>
       <c r="E77" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F77" s="12">
         <v>2</v>
@@ -4442,10 +4423,10 @@
     </row>
     <row r="78" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C78" s="11">
         <v>44411</v>
@@ -4454,7 +4435,7 @@
         <v>10</v>
       </c>
       <c r="E78" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F78" s="12">
         <v>3</v>
@@ -4471,10 +4452,10 @@
     </row>
     <row r="79" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C79" s="11">
         <v>44411</v>
@@ -4483,7 +4464,7 @@
         <v>10</v>
       </c>
       <c r="E79" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F79" s="12">
         <v>4</v>
@@ -4500,10 +4481,10 @@
     </row>
     <row r="80" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C80" s="11">
         <v>44411</v>
@@ -4512,7 +4493,7 @@
         <v>10</v>
       </c>
       <c r="E80" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F80" s="12">
         <v>5</v>
@@ -4529,10 +4510,10 @@
     </row>
     <row r="81" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C81" s="11">
         <v>44411</v>
@@ -4541,7 +4522,7 @@
         <v>10</v>
       </c>
       <c r="E81" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F81" s="12">
         <v>6</v>
@@ -4558,10 +4539,10 @@
     </row>
     <row r="82" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C82" s="11">
         <v>44411</v>
@@ -4570,7 +4551,7 @@
         <v>10</v>
       </c>
       <c r="E82" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F82" s="12">
         <v>7</v>
@@ -4587,10 +4568,10 @@
     </row>
     <row r="83" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C83" s="11">
         <v>44411</v>
@@ -4599,7 +4580,7 @@
         <v>10</v>
       </c>
       <c r="E83" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F83" s="12">
         <v>8</v>
@@ -4616,10 +4597,10 @@
     </row>
     <row r="84" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C84" s="11">
         <v>44411</v>
@@ -4628,7 +4609,7 @@
         <v>10</v>
       </c>
       <c r="E84" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F84" s="12">
         <v>9</v>
@@ -4645,10 +4626,10 @@
     </row>
     <row r="85" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C85" s="11">
         <v>44411</v>
@@ -4657,7 +4638,7 @@
         <v>10</v>
       </c>
       <c r="E85" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F85" s="12">
         <v>10</v>
@@ -4785,169 +4766,169 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="AC4" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="AC5" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="AC6" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>